<commit_message>
completed mesh refinement study, see mesh_refinement_20120305.xlsx
</commit_message>
<xml_diff>
--- a/monoplane_spar_constload/untwisted/mesh_refinement_20120305.xlsx
+++ b/monoplane_spar_constload/untwisted/mesh_refinement_20120305.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>grid density</t>
   </si>
@@ -24,19 +24,41 @@
     <t>tip displacement [m], under static uniform load</t>
   </si>
   <si>
-    <t>(see svy_disp_spar.mdt, column 4, last row)</t>
-  </si>
-  <si>
     <t># of 3rd-order beam elements</t>
   </si>
   <si>
-    <t>1?</t>
+    <t>sw_foam_ielem</t>
+  </si>
+  <si>
+    <t>sc_ielem</t>
+  </si>
+  <si>
+    <t>% difference</t>
+  </si>
+  <si>
+    <t>grid_density_3</t>
+  </si>
+  <si>
+    <t>grid_density_2</t>
+  </si>
+  <si>
+    <t>grid_density_1</t>
+  </si>
+  <si>
+    <t>grid_density_0</t>
+  </si>
+  <si>
+    <t>&lt;--(see svy_disp_spar.mdt, column 4, last row)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000000000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0000000%"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,7 +96,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -88,21 +110,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
+  <cellStyles count="4">
+    <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -112,6 +138,507 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000000E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.56387042917889996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56386726787800001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56385624898730002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56386291455399995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="105797120"/>
+        <c:axId val="105799040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="105797120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="12"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:rPr>
+                  <a:t># cells across foam core thickness</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="105799040"/>
+        <c:crossesAt val="-0.56387200000000004"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="105799040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:rPr>
+                  <a:t>tip displacement [m]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00000E+00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="105797120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.6064314359396628E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.5147961067193898E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.3326864668093274E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="105831424"/>
+        <c:axId val="105841792"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="105831424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="12"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="1"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
+                  <a:t># cells across foam core thickness</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="105841792"/>
+        <c:crossesAt val="-2.5000000000000005E-3"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="105841792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr sz="1600" b="1"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
+                  <a:t>% difference in tip displacement</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0000%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="105831424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr algn="ctr">
+        <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>638174</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -401,47 +928,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
         <v>23</v>
       </c>
-      <c r="C2" s="3">
-        <v>-0.46867071967610002</v>
+      <c r="E2" s="3">
+        <v>0.56387042917889996</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>80</v>
+      </c>
+      <c r="D3">
+        <v>23</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.56386726787800001</v>
+      </c>
+      <c r="G3" s="4">
+        <f>(E3-$E$2)/$E$2</f>
+        <v>-5.6064314359396628E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.56385624898730002</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" ref="G4:G5" si="0">(E4-$E$2)/$E$2</f>
+        <v>-2.5147961067193898E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>120</v>
+      </c>
+      <c r="D5">
+        <v>23</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.56386291455399995</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>-1.3326864668093274E-5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
removed borders on graphs from mesh refinement study
</commit_message>
<xml_diff>
--- a/monoplane_spar_constload/untwisted/mesh_refinement_20120305.xlsx
+++ b/monoplane_spar_constload/untwisted/mesh_refinement_20120305.xlsx
@@ -231,11 +231,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="105797120"/>
-        <c:axId val="105799040"/>
+        <c:axId val="84042880"/>
+        <c:axId val="84045184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105797120"/>
+        <c:axId val="84042880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -297,12 +297,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105799040"/>
+        <c:crossAx val="84045184"/>
         <c:crossesAt val="-0.56387200000000004"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105799040"/>
+        <c:axId val="84045184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -355,7 +355,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105797120"/>
+        <c:crossAx val="84042880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -364,6 +364,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -463,11 +468,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="105831424"/>
-        <c:axId val="105841792"/>
+        <c:axId val="84068992"/>
+        <c:axId val="84079744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105831424"/>
+        <c:axId val="84068992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -498,12 +503,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105841792"/>
+        <c:crossAx val="84079744"/>
         <c:crossesAt val="-2.5000000000000005E-3"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105841792"/>
+        <c:axId val="84079744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,7 +547,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105831424"/>
+        <c:crossAx val="84068992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -551,6 +556,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>

</xml_diff>